<commit_message>
senseBe_rev4 PCB layout done.
</commit_message>
<xml_diff>
--- a/senseBe_rev4/senseBe_rev4_main/senseBe_rev4_main.xlsx
+++ b/senseBe_rev4/senseBe_rev4_main/senseBe_rev4_main.xlsx
@@ -13,10 +13,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1570103695" val="971" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1570103695" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1570103695"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1570103695"/>
+      <pm:revision xmlns:pm="smNativeData" day="1571054021" val="971" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1571054021" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1571054021"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1571054021"/>
     </ext>
   </extLst>
 </workbook>
@@ -85,13 +85,13 @@
     <t xml:space="preserve">C5 C7 C9 </t>
   </si>
   <si>
-    <t>"100nF"</t>
+    <t>"0.1uF"</t>
   </si>
   <si>
     <t xml:space="preserve">C6 </t>
   </si>
   <si>
-    <t>"10Uf"</t>
+    <t>"10uF"</t>
   </si>
   <si>
     <t>"Capacitor_SMD:C_0805_2012Metric"</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">C8 </t>
   </si>
   <si>
-    <t>"10u"</t>
+    <t>"22uF"</t>
   </si>
   <si>
     <t xml:space="preserve">D1 </t>
@@ -318,7 +318,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -326,7 +326,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1570103695" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1571054021" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -334,16 +334,43 @@
         </ext>
       </extLst>
     </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1571054021" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="200" lang="default"/>
+            <pm:ea face="SimSun" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1571054021" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -359,7 +386,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1570103695"/>
+          <pm:border xmlns:pm="smNativeData" id="1571054021"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1571054021"/>
         </ext>
       </extLst>
     </border>
@@ -367,8 +413,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -376,7 +428,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1570103695" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1571054021" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -640,596 +692,597 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:XFD34"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="20.20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.693694" customWidth="1" style="0"/>
-    <col min="2" max="2" width="8.027027" customWidth="1" style="0"/>
-    <col min="3" max="3" width="19.756757" customWidth="1" style="0"/>
-    <col min="4" max="4" width="56.909910" customWidth="1" style="0"/>
-    <col min="5" max="5" width="47.747748" customWidth="1" style="0"/>
+    <col min="1" max="1" width="34.693694" customWidth="1" style="1"/>
+    <col min="2" max="2" width="8.027027" customWidth="1" style="1"/>
+    <col min="3" max="3" width="29.351351" customWidth="1" style="1"/>
+    <col min="4" max="4" width="30.504505" customWidth="1" style="1"/>
+    <col min="5" max="5" width="13.648649" customWidth="1" style="1"/>
+    <col min="6" max="16384" width="10.000000" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16384" s="2" customFormat="1" ht="15.70" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+    <row r="22" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
+    <row r="24" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B26" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
+    <row r="28" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
+    <row r="30" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B30" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
+    <row r="31" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
+    <row r="33" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="20.20" customHeight="1">
+      <c r="A34" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B34" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1237,7 +1290,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1570103695" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1571054021" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1246,16 +1299,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1570103695" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1570103695" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1570103695" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1570103695" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1571054021" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1571054021" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1571054021" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1571054021" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1570103695" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1571054021" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>